<commit_message>
Develop utilities to create a Matrix and multiply matrices
</commit_message>
<xml_diff>
--- a/test/data.xlsx
+++ b/test/data.xlsx
@@ -8,26 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Balli\OneDrive\Desktop\supply-chain\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F99B229E-BD2B-4180-BED0-00B0CEF87544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA189D9-4800-4DEB-B3D7-A5AF481FAC70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3290" yWindow="2790" windowWidth="28800" windowHeight="15370" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45700" yWindow="1840" windowWidth="23770" windowHeight="14930" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="1" r:id="rId1"/>
     <sheet name="forecast" sheetId="2" r:id="rId2"/>
-    <sheet name="routings" sheetId="3" r:id="rId3"/>
+    <sheet name="requirements" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="23">
   <si>
     <t>item</t>
   </si>
@@ -35,12 +46,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>cost</t>
-  </si>
-  <si>
-    <t>price</t>
-  </si>
-  <si>
     <t>item1</t>
   </si>
   <si>
@@ -62,26 +67,53 @@
     <t>resource</t>
   </si>
   <si>
-    <t>requirement</t>
-  </si>
-  <si>
-    <t>resource1</t>
-  </si>
-  <si>
-    <t>resource2</t>
-  </si>
-  <si>
-    <t>resouce3</t>
-  </si>
-  <si>
-    <t>resource4</t>
+    <t>machine1</t>
+  </si>
+  <si>
+    <t>machine2</t>
+  </si>
+  <si>
+    <t>machine3</t>
+  </si>
+  <si>
+    <t>machine4</t>
+  </si>
+  <si>
+    <t>labor1</t>
+  </si>
+  <si>
+    <t>labor2</t>
+  </si>
+  <si>
+    <t>item3</t>
+  </si>
+  <si>
+    <t>item5</t>
+  </si>
+  <si>
+    <t>item4</t>
+  </si>
+  <si>
+    <t>Raw material</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>Flagship Packaging</t>
+  </si>
+  <si>
+    <t>item6</t>
+  </si>
+  <si>
+    <t>Economy Packaging</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +127,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -104,7 +144,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -112,12 +152,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,57 +448,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
-        <v>10</v>
-      </c>
-      <c r="D2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>7</v>
-      </c>
-      <c r="D3">
-        <v>9.5</v>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -461,25 +525,25 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection sqref="A1:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>202301</v>
@@ -490,7 +554,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>202302</v>
@@ -501,7 +565,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>202303</v>
@@ -512,7 +576,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>202304</v>
@@ -523,7 +587,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B6">
         <v>202305</v>
@@ -534,7 +598,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B7">
         <v>202306</v>
@@ -545,7 +609,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B8">
         <v>202307</v>
@@ -556,7 +620,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B9">
         <v>202308</v>
@@ -567,7 +631,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B10">
         <v>202309</v>
@@ -578,7 +642,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B11">
         <v>202310</v>
@@ -589,7 +653,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B12">
         <v>202311</v>
@@ -600,7 +664,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B13">
         <v>202312</v>
@@ -611,7 +675,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B14">
         <v>202301</v>
@@ -622,7 +686,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B15">
         <v>202302</v>
@@ -633,7 +697,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B16">
         <v>202303</v>
@@ -644,7 +708,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B17">
         <v>202304</v>
@@ -655,7 +719,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B18">
         <v>202305</v>
@@ -666,7 +730,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B19">
         <v>202306</v>
@@ -677,7 +741,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B20">
         <v>202307</v>
@@ -688,7 +752,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B21">
         <v>202308</v>
@@ -699,7 +763,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B22">
         <v>202309</v>
@@ -710,7 +774,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B23">
         <v>202310</v>
@@ -721,7 +785,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B24">
         <v>202311</v>
@@ -732,7 +796,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B25">
         <v>202312</v>
@@ -749,10 +813,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{959B0A25-8181-4FB6-BFC1-26D645F901FD}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -761,81 +825,126 @@
     <col min="3" max="3" width="19.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C9">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
         <v>13</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7">
-        <v>1.25</v>
+      <c r="C10">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11">
+        <v>0.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the generateInventoryPlan utility, generateBuildPlan utility is a work in progress
Saving progress to stop for the night.
</commit_message>
<xml_diff>
--- a/test/data.xlsx
+++ b/test/data.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Balli\OneDrive\Desktop\supply-chain\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ABDE2B9-AC09-46D6-8513-6F6145C63578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A47AA83-2C32-4F7D-B13A-221AB80CC93F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6510" yWindow="3000" windowWidth="28800" windowHeight="15370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="1" r:id="rId1"/>
-    <sheet name="resources" sheetId="5" r:id="rId2"/>
-    <sheet name="forecast" sheetId="2" r:id="rId3"/>
-    <sheet name="requirements" sheetId="3" r:id="rId4"/>
-    <sheet name="capacities" sheetId="4" r:id="rId5"/>
+    <sheet name="inventory" sheetId="6" r:id="rId2"/>
+    <sheet name="resources" sheetId="5" r:id="rId3"/>
+    <sheet name="forecast" sheetId="2" r:id="rId4"/>
+    <sheet name="requirements" sheetId="3" r:id="rId5"/>
+    <sheet name="constraints" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="27">
   <si>
     <t>item</t>
   </si>
@@ -48,9 +49,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>quantity</t>
-  </si>
-  <si>
     <t>resource</t>
   </si>
   <si>
@@ -106,6 +104,24 @@
   </si>
   <si>
     <t>period</t>
+  </si>
+  <si>
+    <t>safetyStock</t>
+  </si>
+  <si>
+    <t>levelLoad</t>
+  </si>
+  <si>
+    <t>requirement</t>
+  </si>
+  <si>
+    <t>forecast</t>
+  </si>
+  <si>
+    <t>constraint</t>
+  </si>
+  <si>
+    <t>inventory</t>
   </si>
 </sst>
 </file>
@@ -164,10 +180,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,79 +465,129 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="83.6328125" customWidth="1"/>
+    <col min="3" max="3" width="11.36328125" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>43336</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+      <c r="C2">
+        <v>0.46</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>43337</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <v>0.46</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>43338</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>0.92</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>43339</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+      <c r="C5">
+        <v>0.46</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>40717</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+      <c r="C6">
+        <v>0.46</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>40718</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+      <c r="C7">
+        <v>0.46</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>40200</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -529,11 +596,90 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00DBFAF6-4BC5-41B1-8102-8B95E6FF42BD}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>43336</v>
+      </c>
+      <c r="B2" s="2">
+        <v>33760</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>43337</v>
+      </c>
+      <c r="B3" s="2">
+        <v>18539</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>43338</v>
+      </c>
+      <c r="B4" s="2">
+        <v>2929</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>43339</v>
+      </c>
+      <c r="B5" s="2">
+        <v>12550</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>40717</v>
+      </c>
+      <c r="B6" s="2">
+        <v>15032</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>40718</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2986</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>40200</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1008</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CD610E2-C29B-4C20-B7B6-F7B1729B5B3B}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A4"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -544,7 +690,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -552,34 +698,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -587,12 +733,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65CEA5BC-DEE7-42CC-81EB-835BD67FFC70}">
   <dimension ref="A1:R85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33:C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -602,10 +748,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
@@ -1582,12 +1728,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{959B0A25-8181-4FB6-BFC1-26D645F901FD}">
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1602,13 +1748,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -1616,13 +1762,13 @@
         <v>43336</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>3.676E-3</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -1630,13 +1776,13 @@
         <v>43336</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>3.637E-3</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -1644,13 +1790,13 @@
         <v>43336</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>3.676E-3</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -1658,14 +1804,14 @@
         <v>43336</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <f>0.003677*2</f>
         <v>7.3540000000000003E-3</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -1673,13 +1819,13 @@
         <v>43337</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>3.676E-3</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -1687,13 +1833,13 @@
         <v>43337</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>3.637E-3</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -1701,13 +1847,13 @@
         <v>43337</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <v>3.676E-3</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -1715,14 +1861,14 @@
         <v>43337</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9">
         <f>0.003677*2</f>
         <v>7.3540000000000003E-3</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -1730,13 +1876,13 @@
         <v>43338</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10">
         <v>4.751E-3</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -1744,13 +1890,13 @@
         <v>43338</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <v>4.751E-3</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -1758,13 +1904,13 @@
         <v>43338</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12">
         <v>4.751E-3</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -1772,14 +1918,14 @@
         <v>43338</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13">
         <f>0.004751*2</f>
         <v>9.502E-3</v>
       </c>
       <c r="D13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
@@ -1787,13 +1933,13 @@
         <v>43339</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14">
         <v>3.676E-3</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
@@ -1801,13 +1947,13 @@
         <v>43339</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15">
         <v>3.637E-3</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
@@ -1815,13 +1961,13 @@
         <v>43339</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16">
         <v>3.676E-3</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
@@ -1829,14 +1975,14 @@
         <v>43339</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C17">
         <f>0.003677*2</f>
         <v>7.3540000000000003E-3</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
@@ -1844,13 +1990,13 @@
         <v>40717</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C18">
         <v>3.676E-3</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
@@ -1858,13 +2004,13 @@
         <v>40717</v>
       </c>
       <c r="B19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C19">
         <v>3.637E-3</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
@@ -1872,13 +2018,13 @@
         <v>40717</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C20">
         <v>3.676E-3</v>
       </c>
       <c r="D20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
@@ -1886,14 +2032,14 @@
         <v>40717</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21">
         <f>0.003677*2</f>
         <v>7.3540000000000003E-3</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
@@ -1901,13 +2047,13 @@
         <v>40718</v>
       </c>
       <c r="B22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C22">
         <v>3.676E-3</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
@@ -1915,13 +2061,13 @@
         <v>40718</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C23">
         <v>3.637E-3</v>
       </c>
       <c r="D23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
@@ -1929,13 +2075,13 @@
         <v>40718</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C24">
         <v>3.676E-3</v>
       </c>
       <c r="D24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
@@ -1943,14 +2089,14 @@
         <v>40718</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C25">
         <f>0.003677*2</f>
         <v>7.3540000000000003E-3</v>
       </c>
       <c r="D25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
@@ -1958,13 +2104,13 @@
         <v>40200</v>
       </c>
       <c r="B26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C26">
         <v>4.751E-3</v>
       </c>
       <c r="D26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
@@ -1972,13 +2118,13 @@
         <v>40200</v>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C27">
         <v>4.751E-3</v>
       </c>
       <c r="D27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
@@ -1986,13 +2132,13 @@
         <v>40200</v>
       </c>
       <c r="B28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C28">
         <v>4.751E-3</v>
       </c>
       <c r="D28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
@@ -2000,14 +2146,14 @@
         <v>40200</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C29">
         <f>0.004751*2</f>
         <v>9.502E-3</v>
       </c>
       <c r="D29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2027,25 +2173,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E099F10-FA1B-43D2-A786-45F554B217C9}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Creating function to generate Horizontal Plans
</commit_message>
<xml_diff>
--- a/test/data.xlsx
+++ b/test/data.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Balli\OneDrive\Desktop\supply-chain\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A47AA83-2C32-4F7D-B13A-221AB80CC93F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F70E9B-1468-42D9-9705-10E5FAD9DE64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6510" yWindow="3000" windowWidth="28800" windowHeight="15370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="1140" windowWidth="20700" windowHeight="13180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="1" r:id="rId1"/>
-    <sheet name="inventory" sheetId="6" r:id="rId2"/>
-    <sheet name="resources" sheetId="5" r:id="rId3"/>
-    <sheet name="forecast" sheetId="2" r:id="rId4"/>
-    <sheet name="requirements" sheetId="3" r:id="rId5"/>
-    <sheet name="constraints" sheetId="4" r:id="rId6"/>
+    <sheet name="resources" sheetId="5" r:id="rId2"/>
+    <sheet name="forecast" sheetId="2" r:id="rId3"/>
+    <sheet name="requirements" sheetId="3" r:id="rId4"/>
+    <sheet name="constraints" sheetId="4" r:id="rId5"/>
+    <sheet name="calendar" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="34">
   <si>
     <t>item</t>
   </si>
@@ -109,9 +109,6 @@
     <t>safetyStock</t>
   </si>
   <si>
-    <t>levelLoad</t>
-  </si>
-  <si>
     <t>requirement</t>
   </si>
   <si>
@@ -121,7 +118,31 @@
     <t>constraint</t>
   </si>
   <si>
-    <t>inventory</t>
+    <t>FOQ</t>
+  </si>
+  <si>
+    <t>palletQty</t>
+  </si>
+  <si>
+    <t>days</t>
+  </si>
+  <si>
+    <t>startDate</t>
+  </si>
+  <si>
+    <t>Make-to-Order</t>
+  </si>
+  <si>
+    <t>Reactive Level Load - Fast</t>
+  </si>
+  <si>
+    <t>Reactive Level Load - Slow</t>
+  </si>
+  <si>
+    <t>strategy</t>
+  </si>
+  <si>
+    <t>currentInventory</t>
   </si>
 </sst>
 </file>
@@ -184,7 +205,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,20 +486,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="83.6328125" customWidth="1"/>
     <col min="3" max="3" width="11.36328125" customWidth="1"/>
-    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="4" max="4" width="27.453125" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -489,10 +511,19 @@
         <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>43336</v>
       </c>
@@ -502,11 +533,20 @@
       <c r="C2">
         <v>0.46</v>
       </c>
-      <c r="D2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="2">
+        <v>33760</v>
+      </c>
+      <c r="F2">
+        <v>2772</v>
+      </c>
+      <c r="G2">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>43337</v>
       </c>
@@ -516,11 +556,20 @@
       <c r="C3">
         <v>0.46</v>
       </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="2">
+        <v>18539</v>
+      </c>
+      <c r="F3">
+        <v>2772</v>
+      </c>
+      <c r="G3">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>43338</v>
       </c>
@@ -530,11 +579,20 @@
       <c r="C4">
         <v>0.92</v>
       </c>
-      <c r="D4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2929</v>
+      </c>
+      <c r="F4">
+        <v>2520</v>
+      </c>
+      <c r="G4">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>43339</v>
       </c>
@@ -544,11 +602,20 @@
       <c r="C5">
         <v>0.46</v>
       </c>
-      <c r="D5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="2">
+        <v>12550</v>
+      </c>
+      <c r="F5">
+        <v>2772</v>
+      </c>
+      <c r="G5">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>40717</v>
       </c>
@@ -558,11 +625,20 @@
       <c r="C6">
         <v>0.46</v>
       </c>
-      <c r="D6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="2">
+        <v>15032</v>
+      </c>
+      <c r="F6">
+        <v>2772</v>
+      </c>
+      <c r="G6">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>40718</v>
       </c>
@@ -572,11 +648,20 @@
       <c r="C7">
         <v>0.46</v>
       </c>
-      <c r="D7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2986</v>
+      </c>
+      <c r="F7">
+        <v>2772</v>
+      </c>
+      <c r="G7">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>40200</v>
       </c>
@@ -586,8 +671,17 @@
       <c r="C8">
         <v>0</v>
       </c>
-      <c r="D8" t="b">
-        <v>0</v>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1008</v>
+      </c>
+      <c r="F8">
+        <v>2520</v>
+      </c>
+      <c r="G8">
+        <v>504</v>
       </c>
     </row>
   </sheetData>
@@ -596,85 +690,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00DBFAF6-4BC5-41B1-8102-8B95E6FF42BD}">
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>43336</v>
-      </c>
-      <c r="B2" s="2">
-        <v>33760</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>43337</v>
-      </c>
-      <c r="B3" s="2">
-        <v>18539</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>43338</v>
-      </c>
-      <c r="B4" s="2">
-        <v>2929</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>43339</v>
-      </c>
-      <c r="B5" s="2">
-        <v>12550</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>40717</v>
-      </c>
-      <c r="B6" s="2">
-        <v>15032</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>40718</v>
-      </c>
-      <c r="B7" s="2">
-        <v>2986</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>40200</v>
-      </c>
-      <c r="B8" s="2">
-        <v>1008</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CD610E2-C29B-4C20-B7B6-F7B1729B5B3B}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -733,12 +748,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65CEA5BC-DEE7-42CC-81EB-835BD67FFC70}">
   <dimension ref="A1:R85"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:C33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -751,7 +766,7 @@
         <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
@@ -1728,12 +1743,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{959B0A25-8181-4FB6-BFC1-26D645F901FD}">
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1751,7 +1766,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>12</v>
@@ -2173,17 +2188,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E099F10-FA1B-43D2-A786-45F554B217C9}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="D2" sqref="D2:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2191,10 +2206,10 @@
         <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>41159</v>
       </c>
@@ -2204,8 +2219,12 @@
       <c r="C2">
         <v>380</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2">
+        <f>C2/20</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>41159</v>
       </c>
@@ -2215,8 +2234,12 @@
       <c r="C3">
         <v>300</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D3">
+        <f t="shared" ref="D3:D13" si="0">C3/20</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>41159</v>
       </c>
@@ -2226,8 +2249,12 @@
       <c r="C4">
         <v>360</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>41159</v>
       </c>
@@ -2238,8 +2265,12 @@
         <f>17*20</f>
         <v>340</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>41159</v>
       </c>
@@ -2250,8 +2281,12 @@
         <f>14*20</f>
         <v>280</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>41159</v>
       </c>
@@ -2262,8 +2297,12 @@
         <f>18*20</f>
         <v>360</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>41159</v>
       </c>
@@ -2274,8 +2313,12 @@
         <f>17*20</f>
         <v>340</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>41159</v>
       </c>
@@ -2285,8 +2328,12 @@
       <c r="C9">
         <v>320</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>41159</v>
       </c>
@@ -2297,8 +2344,12 @@
         <f>17*20</f>
         <v>340</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>41159</v>
       </c>
@@ -2309,8 +2360,12 @@
         <f>17*20</f>
         <v>340</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>41159</v>
       </c>
@@ -2321,8 +2376,12 @@
         <f>16*20</f>
         <v>320</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>41159</v>
       </c>
@@ -2332,6 +2391,171 @@
       <c r="C13">
         <f>18*20</f>
         <v>360</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8472E45-B98D-4B8B-9BC0-59A0B23E2756}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>202308</v>
+      </c>
+      <c r="B2" s="3">
+        <v>45139</v>
+      </c>
+      <c r="C2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>202309</v>
+      </c>
+      <c r="B3" s="3">
+        <v>45170</v>
+      </c>
+      <c r="C3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>202310</v>
+      </c>
+      <c r="B4" s="3">
+        <v>45200</v>
+      </c>
+      <c r="C4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>202311</v>
+      </c>
+      <c r="B5" s="3">
+        <v>45231</v>
+      </c>
+      <c r="C5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>202312</v>
+      </c>
+      <c r="B6" s="3">
+        <v>45261</v>
+      </c>
+      <c r="C6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>202401</v>
+      </c>
+      <c r="B7" s="3">
+        <v>45292</v>
+      </c>
+      <c r="C7">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>202402</v>
+      </c>
+      <c r="B8" s="3">
+        <v>45323</v>
+      </c>
+      <c r="C8">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>202403</v>
+      </c>
+      <c r="B9" s="3">
+        <v>45352</v>
+      </c>
+      <c r="C9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>202404</v>
+      </c>
+      <c r="B10" s="3">
+        <v>45383</v>
+      </c>
+      <c r="C10">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>202405</v>
+      </c>
+      <c r="B11" s="3">
+        <v>45413</v>
+      </c>
+      <c r="C11">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>202406</v>
+      </c>
+      <c r="B12" s="3">
+        <v>45444</v>
+      </c>
+      <c r="C12">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>202407</v>
+      </c>
+      <c r="B13" s="3">
+        <v>45474</v>
+      </c>
+      <c r="C13">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed initial build of Planning View Generator
</commit_message>
<xml_diff>
--- a/test/data.xlsx
+++ b/test/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Balli\OneDrive\Desktop\supply-chain\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F70E9B-1468-42D9-9705-10E5FAD9DE64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89880AD6-52D6-4C44-9EEA-54469A034DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1140" windowWidth="20700" windowHeight="13180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2660" yWindow="2660" windowWidth="28800" windowHeight="15370" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="items" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="36">
   <si>
     <t>item</t>
   </si>
@@ -106,9 +106,6 @@
     <t>period</t>
   </si>
   <si>
-    <t>safetyStock</t>
-  </si>
-  <si>
     <t>requirement</t>
   </si>
   <si>
@@ -143,6 +140,15 @@
   </si>
   <si>
     <t>currentInventory</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>Machine</t>
+  </si>
+  <si>
+    <t>Labor</t>
   </si>
 </sst>
 </file>
@@ -486,21 +492,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="83.6328125" customWidth="1"/>
-    <col min="3" max="3" width="11.36328125" customWidth="1"/>
-    <col min="4" max="4" width="27.453125" customWidth="1"/>
-    <col min="5" max="5" width="8.7265625" customWidth="1"/>
+    <col min="3" max="3" width="27.453125" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -508,179 +513,155 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>43336</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="C2">
-        <v>0.46</v>
-      </c>
-      <c r="D2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="2">
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="2">
         <v>33760</v>
       </c>
+      <c r="E2">
+        <v>2772</v>
+      </c>
       <c r="F2">
-        <v>2772</v>
-      </c>
-      <c r="G2">
         <v>504</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>43337</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="C3">
-        <v>0.46</v>
-      </c>
-      <c r="D3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="2">
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="2">
         <v>18539</v>
       </c>
+      <c r="E3">
+        <v>2772</v>
+      </c>
       <c r="F3">
-        <v>2772</v>
-      </c>
-      <c r="G3">
         <v>504</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>43338</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="C4">
-        <v>0.92</v>
-      </c>
-      <c r="D4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="2">
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="2">
         <v>2929</v>
       </c>
+      <c r="E4">
+        <v>2520</v>
+      </c>
       <c r="F4">
-        <v>2520</v>
-      </c>
-      <c r="G4">
         <v>504</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>43339</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="C5">
-        <v>0.46</v>
-      </c>
-      <c r="D5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="2">
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="2">
         <v>12550</v>
       </c>
+      <c r="E5">
+        <v>2772</v>
+      </c>
       <c r="F5">
-        <v>2772</v>
-      </c>
-      <c r="G5">
         <v>504</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>40717</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c r="C6">
-        <v>0.46</v>
-      </c>
-      <c r="D6" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="2">
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="2">
         <v>15032</v>
       </c>
+      <c r="E6">
+        <v>2772</v>
+      </c>
       <c r="F6">
-        <v>2772</v>
-      </c>
-      <c r="G6">
         <v>504</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>40718</v>
       </c>
       <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="C7">
-        <v>0.46</v>
-      </c>
-      <c r="D7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="2">
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="2">
         <v>2986</v>
       </c>
+      <c r="E7">
+        <v>2772</v>
+      </c>
       <c r="F7">
-        <v>2772</v>
-      </c>
-      <c r="G7">
         <v>504</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>40200</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="2">
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="2">
         <v>1008</v>
       </c>
+      <c r="E8">
+        <v>2520</v>
+      </c>
       <c r="F8">
-        <v>2520</v>
-      </c>
-      <c r="G8">
         <v>504</v>
       </c>
     </row>
@@ -691,10 +672,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CD610E2-C29B-4C20-B7B6-F7B1729B5B3B}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -703,44 +684,59 @@
     <col min="2" max="2" width="33.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -766,7 +762,7 @@
         <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
@@ -1766,7 +1762,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>12</v>
@@ -2190,15 +2186,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E099F10-FA1B-43D2-A786-45F554B217C9}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2206,10 +2202,10 @@
         <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>41159</v>
       </c>
@@ -2219,12 +2215,8 @@
       <c r="C2">
         <v>380</v>
       </c>
-      <c r="D2">
-        <f>C2/20</f>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>41159</v>
       </c>
@@ -2234,12 +2226,8 @@
       <c r="C3">
         <v>300</v>
       </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D13" si="0">C3/20</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>41159</v>
       </c>
@@ -2249,12 +2237,8 @@
       <c r="C4">
         <v>360</v>
       </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>41159</v>
       </c>
@@ -2265,12 +2249,8 @@
         <f>17*20</f>
         <v>340</v>
       </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>41159</v>
       </c>
@@ -2281,12 +2261,8 @@
         <f>14*20</f>
         <v>280</v>
       </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>41159</v>
       </c>
@@ -2297,12 +2273,8 @@
         <f>18*20</f>
         <v>360</v>
       </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>41159</v>
       </c>
@@ -2313,12 +2285,8 @@
         <f>17*20</f>
         <v>340</v>
       </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>41159</v>
       </c>
@@ -2328,12 +2296,8 @@
       <c r="C9">
         <v>320</v>
       </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>41159</v>
       </c>
@@ -2344,12 +2308,8 @@
         <f>17*20</f>
         <v>340</v>
       </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>41159</v>
       </c>
@@ -2360,12 +2320,8 @@
         <f>17*20</f>
         <v>340</v>
       </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>41159</v>
       </c>
@@ -2376,12 +2332,8 @@
         <f>16*20</f>
         <v>320</v>
       </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>41159</v>
       </c>
@@ -2391,10 +2343,6 @@
       <c r="C13">
         <f>18*20</f>
         <v>360</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -2407,7 +2355,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2420,10 +2368,10 @@
         <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>